<commit_message>
Update cost and robot comparison table
</commit_message>
<xml_diff>
--- a/Latex/Thesis/data/cost_of_parts.xlsx
+++ b/Latex/Thesis/data/cost_of_parts.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="46">
   <si>
     <t xml:space="preserve">Description:</t>
   </si>
@@ -35,6 +35,117 @@
     <t xml:space="preserve">cost (dollar):</t>
   </si>
   <si>
+    <t xml:space="preserve">total cost (dollar):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost for 20 (dollar):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total cost (dollar):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26:1 Sub-Micro Plastic Planetary Gearmotor 6Dx16L mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pololu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wheels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14×4.5mm Wheel Pair for Sub-Micro Plastic Planetary Gearmotors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ball Caster with 1/2″ Plastic Ball</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harvester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BQ25570</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digikey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gyroscope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BMG250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H-bridge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI DRV8836</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supercap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BZ054B223ZSB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mouser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPR board v2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Osh Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solar panel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLMD121H04L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small components</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farnell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Euro price:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extra sensor:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proximity sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAX44000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IR led for proximity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SFH 4651-Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proximity board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL EURO PRICE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost:</t>
+  </si>
+  <si>
     <t xml:space="preserve">total cost:</t>
   </si>
   <si>
@@ -42,108 +153,6 @@
   </si>
   <si>
     <t xml:space="preserve">Total cost:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">From:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26:1 Sub-Micro Plastic Planetary Gearmotor 6Dx16L mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pololu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wheels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14×4.5mm Wheel Pair for Sub-Micro Plastic Planetary Gearmotors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Caster</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ball Caster with 1/2″ Plastic Ball</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harvester</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BQ25570</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digikey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gyroscope</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BMG250</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H-bridge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TI DRV8836</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supercap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BZ054B223ZSB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mouser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IPR board v2.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Osh Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solar panel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SLMD121H04L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Small components</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Farnell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Euro price:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extra sensor:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proximity sensor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAX44000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IR led for proximity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SFH 4651-Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proximity board</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOTAL EURO PRICE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cost:</t>
   </si>
   <si>
     <t xml:space="preserve">Tme.eu</t>
@@ -254,21 +263,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H25" activeCellId="0" sqref="H25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1887755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.5714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.9081632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.2091836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="20.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.9438775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -324,6 +333,10 @@
       <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="I2" s="0" t="n">
+        <f aca="false">G2*0.86</f>
+        <v>18.5072</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -352,6 +365,10 @@
       <c r="H3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="I3" s="0" t="n">
+        <f aca="false">G3*0.86</f>
+        <v>1.5394</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -380,6 +397,10 @@
       <c r="H4" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="I4" s="0" t="n">
+        <f aca="false">G4*0.86</f>
+        <v>1.5394</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -408,6 +429,10 @@
       <c r="H5" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="I5" s="0" t="n">
+        <f aca="false">G5*0.86</f>
+        <v>5.4782</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -436,6 +461,10 @@
       <c r="H6" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="I6" s="0" t="n">
+        <f aca="false">G6*0.86</f>
+        <v>2.8122</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -464,6 +493,10 @@
       <c r="H7" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="I7" s="0" t="n">
+        <f aca="false">G7*0.86</f>
+        <v>1.4792</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -492,6 +525,10 @@
       <c r="H8" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="I8" s="0" t="n">
+        <f aca="false">G8*0.86</f>
+        <v>7.4304</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -522,6 +559,10 @@
       <c r="H9" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="I9" s="0" t="n">
+        <f aca="false">G9*0.86</f>
+        <v>1.86333333333334</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -550,6 +591,10 @@
       <c r="H10" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="I10" s="0" t="n">
+        <f aca="false">G10*0.86</f>
+        <v>9.5976</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -579,6 +624,10 @@
       </c>
       <c r="H11" s="1" t="s">
         <v>31</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <f aca="false">G11*0.86</f>
+        <v>3.78916</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -589,6 +638,10 @@
       <c r="G12" s="1" t="n">
         <f aca="false">SUM(G2:G11)</f>
         <v>62.8326666666667</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <f aca="false">G12*0.86</f>
+        <v>54.0360933333334</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -762,14 +815,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.8826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="58.4489795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="57.7755102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -786,13 +839,13 @@
         <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
@@ -823,7 +876,7 @@
         <v>18.82</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -851,7 +904,7 @@
         <v>1.89</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -879,7 +932,7 @@
         <v>1.83</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1034,7 +1087,7 @@
         <v>28</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>2</v>
@@ -1099,6 +1152,14 @@
         <v>62.3849451476793</v>
       </c>
       <c r="H12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0"/>
+      <c r="B13" s="0"/>
+      <c r="E13" s="0"/>
+      <c r="F13" s="0"/>
+      <c r="G13" s="0"/>
+      <c r="H13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">

</xml_diff>